<commit_message>
change status of document: use case diagram is complete.
</commit_message>
<xml_diff>
--- a/doc/list of documents.xlsx
+++ b/doc/list of documents.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Vision</t>
   </si>
@@ -57,13 +57,16 @@
   </si>
   <si>
     <t>complete</t>
+  </si>
+  <si>
+    <t>ü</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +88,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -122,13 +131,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,7 +426,7 @@
   <dimension ref="B2:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,49 +453,51 @@
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="4"/>
     </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="4"/>
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="4"/>
     </row>
     <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated status of document.
</commit_message>
<xml_diff>
--- a/doc/list of documents.xlsx
+++ b/doc/list of documents.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Vision</t>
   </si>
@@ -131,13 +131,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -426,7 +425,7 @@
   <dimension ref="B2:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,13 +446,15 @@
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -461,43 +462,47 @@
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="3"/>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="3"/>
     </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="3"/>
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="3"/>
     </row>
     <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>